<commit_message>
made changes in applied.xlsx file
</commit_message>
<xml_diff>
--- a/project-atlas/data/applied.xlsx
+++ b/project-atlas/data/applied.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,30 +429,35 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>Platform</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Company</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Role</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Location</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -461,35 +466,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>19-01-26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>04:48</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>LinkedIn</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Test Company Ltd</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Junior Software Engineer</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Needs Manual Review</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/jobs/search/?currentJobId=4354716964&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
         </is>
@@ -498,35 +508,40 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>19-01-26</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>04:48</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>LinkedIn</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Test Company Ltd</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Junior Software Engineer</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Needs Manual Review</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/jobs/search/?currentJobId=4363664206&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
         </is>

</xml_diff>

<commit_message>
applying easy apply jobs
</commit_message>
<xml_diff>
--- a/project-atlas/data/applied.xlsx
+++ b/project-atlas/data/applied.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,40 +424,45 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Role</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Platform</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Platform</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Company</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Role</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Location</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -466,84 +471,188 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Test Company Ltd</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Junior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Manual Review</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Timeout 30000ms exceeded.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>19-01-26</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>04:48</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>LinkedIn</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Test Company Ltd</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Junior Software Engineer</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Ireland</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Needs Manual Review</t>
-        </is>
-      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/search/?currentJobId=4354716964&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4364382406&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Test Company Ltd</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Junior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Manual Review</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Timeout 30000ms exceeded.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>19-01-26</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>04:48</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>18:01</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4364203279&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Test Company Ltd</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Junior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>LinkedIn</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Manual Review</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Timeout 30000ms exceeded.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>19-01-26</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4364382406&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Test Company Ltd</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Junior Software Engineer</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Needs Manual Review</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/search/?currentJobId=4363664206&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Manual Review</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Timeout 30000ms exceeded.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>19-01-26</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>18:06</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4364203279&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Basic automation of easy apply jobs working perfectly
</commit_message>
<xml_diff>
--- a/project-atlas/data/applied.xlsx
+++ b/project-atlas/data/applied.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -496,7 +496,13 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Timeout 30000ms exceeded.</t>
+          <t xml:space="preserve">Locator.click: Error: strict mode violation: locator("button:has-text('Next')") resolved to 3 elements:
+    1) &lt;button id="ember359" type="button" data-easy-apply-next-button="" aria-label="Continue to next step" data-live-test-easy-apply-next-button="" class="artdeco-button artdeco-button--2 artdeco-button--primary ember-view"&gt;…&lt;/button&gt; aka get_by_role("button", name="Continue to next step")
+    2) &lt;button id="ember270" type="button" aria-label="View next page" class="artdeco-button artdeco-button--muted artdeco-button--icon-right artdeco-button--1 artdeco-button--tertiary ember-view jobs-search-pagination__button jobs-search-pagination__button--next"&gt;…&lt;/button&gt; aka get_by_label("View next page")
+    3) &lt;button id="ember313" type="button" aria-label="Company photos Next" data-control-name="COMPANY_LIFE_COMPANY_PHOTOS_NEXT" class="artdeco-button artdeco-button--circle artdeco-button--muted artdeco-button--icon-right artdeco-button--1 artdeco-button--tertiary ember-view artdeco-pagination__button artdeco-pagination__button--next"&gt;…&lt;/button&gt; aka get_by_label("Company photos Next")
+Call log:
+  - waiting for locator("button:has-text('Next')")
+</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -506,7 +512,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -543,7 +549,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Timeout 30000ms exceeded.</t>
+          <t xml:space="preserve">Locator.click: Error: strict mode violation: locator("button:has-text('Next')") resolved to 2 elements:
+    1) &lt;button id="ember375" type="button" data-easy-apply-next-button="" aria-label="Continue to next step" data-live-test-easy-apply-next-button="" class="artdeco-button artdeco-button--2 artdeco-button--primary ember-view"&gt;…&lt;/button&gt; aka get_by_role("button", name="Continue to next step")
+    2) &lt;button id="ember270" type="button" aria-label="View next page" class="artdeco-button artdeco-button--muted artdeco-button--icon-right artdeco-button--1 artdeco-button--tertiary ember-view jobs-search-pagination__button jobs-search-pagination__button--next"&gt;…&lt;/button&gt; aka get_by_label("View next page")
+Call log:
+  - waiting for locator("button:has-text('Next')")
+</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -553,7 +564,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>18:01</t>
+          <t>19:35</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -585,12 +596,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Manual Review</t>
+          <t>Applied</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Timeout 30000ms exceeded.</t>
+          <t>Success</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -600,7 +611,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>19:43</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -632,12 +643,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Manual Review</t>
+          <t>Applied</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Timeout 30000ms exceeded.</t>
+          <t>Success</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -647,7 +658,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>19:44</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">

</xml_diff>

<commit_message>
project compeleted with everthing workig fine only fine tuning is left
</commit_message>
<xml_diff>
--- a/project-atlas/data/applied.xlsx
+++ b/project-atlas/data/applied.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -667,6 +667,429 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Test Company Ltd</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Junior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Skipped</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>No Easy Apply</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>19-01-26</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>21:32</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4323316446&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Test Company Ltd</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Junior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Skipped</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>No Easy Apply</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>19-01-26</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>21:32</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4362486265&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Test Company Ltd</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Junior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Skipped</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>No Easy Apply</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>19-01-26</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4323316446&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Test Company Ltd</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Junior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Skipped</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>No Easy Apply</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>19-01-26</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>21:39</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4362486265&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Test Company Ltd</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Junior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Skipped</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>No Easy Apply</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>19-01-26</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>21:40</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4323316446&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Test Company Ltd</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Junior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Skipped</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>No Easy Apply</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>19-01-26</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>21:40</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4362486265&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Test Company Ltd</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Junior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Skipped</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>No Easy Apply</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>19-01-26</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>21:43</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4323316446&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Test Company Ltd</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Junior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Skipped</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>No Easy Apply</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>19-01-26</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>21:44</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4362486265&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Test Company Ltd</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Junior Software Engineer</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Applied</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>19-01-26</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>22:02</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4354434581&amp;f_AL=true&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland&amp;origin=JOB_SEARCH_PAGE_JOB_FILTER&amp;spellCorrectionEnabled=true</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
linkedIn Bot got smarter now
</commit_message>
<xml_diff>
--- a/project-atlas/data/applied.xlsx
+++ b/project-atlas/data/applied.xlsx
@@ -1,94 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Local Disk\Own Projects\Job Hunting Bot\BOT\Job_Hunting_AI_Bot\project-atlas\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BBDA22-1A44-435C-A9A8-86F0F5F8D487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Platform</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Core Optimisation</t>
-  </si>
-  <si>
-    <t>Full Stack Software Engineer</t>
-  </si>
-  <si>
-    <t>LinkedIn</t>
-  </si>
-  <si>
-    <t>Applied</t>
-  </si>
-  <si>
-    <t>Success</t>
-  </si>
-  <si>
-    <t>20-01-26</t>
-  </si>
-  <si>
-    <t>01:45</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/jobs/search/?currentJobId=4353854807&amp;f_AL=true&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -107,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -409,75 +407,495 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col width="20.44140625" customWidth="1" min="1" max="1"/>
+    <col width="22.88671875" customWidth="1" min="2" max="2"/>
+    <col width="15.5546875" customWidth="1" min="3" max="3"/>
+    <col width="19.33203125" customWidth="1" min="4" max="4"/>
+    <col width="12.21875" customWidth="1" min="5" max="5"/>
+    <col width="25.88671875" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="14.109375" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Role</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Platform</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Core Optimisation</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Full Stack Software Engineer</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Applied</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>20-01-26</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>01:45</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4353854807&amp;f_AL=true&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Core Optimisation</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Full Stack Software Engineer</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Manual Review</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Radio / Dropdown questions detected</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>20-01-26</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>02:25</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4353715994&amp;f_AL=true&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Core Optimisation</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Full Stack Software Engineer</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Skipped</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>No Easy Apply</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>20-01-26</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>02:30</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4358580308&amp;f_AL=true&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Core Optimisation</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Full Stack Software Engineer</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Skipped</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No Easy Apply</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>20-01-26</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>02:31</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4353912265&amp;f_AL=true&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Core Optimisation</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Full Stack Software Engineer</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Manual Review</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Radio / Dropdown questions detected</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>20-01-26</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>02:34</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4353912265&amp;f_AL=true&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Core Optimisation</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Full Stack Software Engineer</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Manual Review</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Radio / Dropdown questions detected</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>20-01-26</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>02:35</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4358580308&amp;f_AL=true&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Core Optimisation</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Full Stack Software Engineer</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Applied</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>20-01-26</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>02:42</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4358580308&amp;f_AL=true&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Core Optimisation</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Full Stack Software Engineer</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Manual Review</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Exceeded step limit</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>20-01-26</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>03:05</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4353912265&amp;f_AL=true&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Core Optimisation</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Full Stack Software Engineer</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Manual Review</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>More Information Needed</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>20-01-26</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>03:10</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4343818234&amp;f_AL=true&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Core Optimisation</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Full Stack Software Engineer</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Applied</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>20-01-26</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>03:13</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/search/?currentJobId=4344112071&amp;f_AL=true&amp;keywords=Junior%20Software%20Engineer%20Ireland&amp;location=Ireland</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a bit of changes
</commit_message>
<xml_diff>
--- a/project-atlas/data/applied.xlsx
+++ b/project-atlas/data/applied.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Local Disk\Own Projects\Job Hunting Bot\BOT\Job_Hunting_AI_Bot\project-atlas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F501A5-4D30-4354-89F9-F45B3FE8AE8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A4DF4E-90C9-4F01-B9EE-D14DF3A40196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -389,7 +389,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>